<commit_message>
Added temperature feature with pyexcel
</commit_message>
<xml_diff>
--- a/weather.xlsx
+++ b/weather.xlsx
@@ -69,10 +69,7 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
+  <cellXfs count="3">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -384,233 +381,224 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D13" activeCellId="0" pane="topLeft" sqref="D13"/>
+      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1025" min="1" style="2" width="10.1133603238866"/>
+    <col customWidth="1" max="1025" min="1" style="1" width="9.4251012145749"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="3">
-      <c r="A1" s="2" t="inlineStr">
+    <row customHeight="1" ht="15" r="1" s="2">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>City</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Temperature</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>C/F</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>0/1</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="2" s="3">
-      <c r="A2" s="2" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="2" s="2">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>Mumbai</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="3" s="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="B2" t="n">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="3" s="2">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>Delhi</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>95</v>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="B3" t="n">
+        <v>91.40000000000001</v>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="D3" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="4" s="3">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="4" s="2">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>Indore</t>
         </is>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="5" s="3">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="B4" t="n">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="5" s="2">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>Jaipur</t>
         </is>
       </c>
-      <c r="B5" s="2" t="n">
-        <v>37</v>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="6" s="3">
-      <c r="A6" s="2" t="inlineStr">
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="6" s="2">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>Bangalore</t>
         </is>
       </c>
-      <c r="B6" s="2" t="n">
-        <v>28.30000000000001</v>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="7" s="3">
-      <c r="A7" s="2" t="inlineStr">
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="7" s="2">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>Chennai</t>
         </is>
       </c>
-      <c r="B7" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="8" s="3">
-      <c r="A8" s="2" t="inlineStr">
+      <c r="B7" t="n">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="8" s="2">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>Hyderabad</t>
         </is>
       </c>
-      <c r="B8" s="2" t="n">
-        <v>26.44</v>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="9" s="3">
-      <c r="A9" s="2" t="inlineStr">
+      <c r="B8" t="n">
+        <v>27.74000000000001</v>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="9" s="2">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>Mysore</t>
         </is>
       </c>
-      <c r="B9" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="10" s="3">
-      <c r="A10" s="2" t="inlineStr">
+      <c r="B9" t="n">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="10" s="2">
+      <c r="A10" s="1" t="inlineStr">
         <is>
           <t>Gangtok</t>
         </is>
       </c>
-      <c r="B10" s="2" t="n">
-        <v>19.99000000000001</v>
-      </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="11" s="3">
-      <c r="A11" s="2" t="inlineStr">
+      <c r="B10" t="n">
+        <v>76.40600000000003</v>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="11" s="2">
+      <c r="A11" s="1" t="inlineStr">
         <is>
           <t>Guwhati</t>
         </is>
       </c>
-      <c r="B11" s="2" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="C11" s="2" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="12" s="3">
-      <c r="A12" s="2" t="inlineStr">
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="12" s="2">
+      <c r="A12" s="1" t="inlineStr">
         <is>
           <t>Dubai</t>
         </is>
       </c>
-      <c r="B12" s="2" t="n">
-        <v>39</v>
-      </c>
-      <c r="C12" s="2" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="D12" s="2" t="n">
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -630,16 +618,16 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B2:B12 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1025" min="1" style="2" width="10.1133603238866"/>
+    <col customWidth="1" max="1025" min="1" style="1" width="9.4251012145749"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="3">
-      <c r="A1" s="2" t="inlineStr">
+    <row customHeight="1" ht="15" r="1" s="2">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>City</t>
         </is>

</xml_diff>